<commit_message>
New API format-MA Team
</commit_message>
<xml_diff>
--- a/MuLAN Details.xlsx
+++ b/MuLAN Details.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\envs\cbm\Codes\phase2_reducedcolumns\Data_merge\API_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mariapps-my.sharepoint.com/personal/ashin_johnson_oceanai_ai/Documents/envs/cbm_test2/smartmaintanace/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31BEFCE0-BCA0-403B-8904-D80D78D782C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{31BEFCE0-BCA0-403B-8904-D80D78D782C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A06E7CE-8867-40D5-AEF2-F3D9F5183147}"/>
   <bookViews>
-    <workbookView xWindow="4995" yWindow="8265" windowWidth="21600" windowHeight="11385" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6780" yWindow="540" windowWidth="21600" windowHeight="11385" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Engine 1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -809,16 +809,16 @@
     <t>ME 1 PISTON AND RINGS NO.6</t>
   </si>
   <si>
-    <t>Exhaust Valve</t>
-  </si>
-  <si>
-    <t>Start of Inj</t>
-  </si>
-  <si>
-    <t>Injection System</t>
-  </si>
-  <si>
-    <t>Combustion Blow-by</t>
+    <t>Injection System Fault</t>
+  </si>
+  <si>
+    <t>Start of Injection Fault</t>
+  </si>
+  <si>
+    <t>Exhaust Valve Fault</t>
+  </si>
+  <si>
+    <t>Blow-by in combustion chamber</t>
   </si>
 </sst>
 </file>
@@ -872,6 +872,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6561,8 +6565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7778BF6-03DE-4A9B-B9B8-C41764207DF0}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6626,7 +6630,7 @@
         <v>98</v>
       </c>
       <c r="H2" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -6652,7 +6656,7 @@
         <v>98</v>
       </c>
       <c r="H3" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -6678,7 +6682,7 @@
         <v>98</v>
       </c>
       <c r="H4" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -6704,7 +6708,7 @@
         <v>98</v>
       </c>
       <c r="H5" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -6730,7 +6734,7 @@
         <v>98</v>
       </c>
       <c r="H6" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -6756,7 +6760,7 @@
         <v>98</v>
       </c>
       <c r="H7" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -7250,7 +7254,7 @@
         <v>57</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -7276,7 +7280,7 @@
         <v>57</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -7302,7 +7306,7 @@
         <v>57</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -9691,8 +9695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E624F993-C72D-4D70-82B2-BB7718A977CB}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9701,7 +9705,7 @@
     <col min="2" max="2" width="31.42578125" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" customWidth="1"/>
     <col min="7" max="7" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -9911,7 +9915,7 @@
         <v>57</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -9937,7 +9941,7 @@
         <v>57</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -9963,7 +9967,7 @@
         <v>57</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -10457,7 +10461,7 @@
         <v>98</v>
       </c>
       <c r="H29" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -10483,7 +10487,7 @@
         <v>98</v>
       </c>
       <c r="H30" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -10509,7 +10513,7 @@
         <v>98</v>
       </c>
       <c r="H31" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -10535,7 +10539,7 @@
         <v>98</v>
       </c>
       <c r="H32" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -10561,7 +10565,7 @@
         <v>98</v>
       </c>
       <c r="H33" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -10587,7 +10591,7 @@
         <v>98</v>
       </c>
       <c r="H34" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>